<commit_message>
Entregable Viernes 20 Dic - Con esto se envió información a reaseguradores
</commit_message>
<xml_diff>
--- a/Parametros Querys.xlsx
+++ b/Parametros Querys.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BC\0. Modelos Python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BC\99 GitHub\Licitacion Reaseguro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8C1CE19-5AD2-4E11-BFA2-FB2D2EB561A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CA1C11A-B8C1-4ABA-96BF-086326126456}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="723" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-3765" windowWidth="29040" windowHeight="15840" tabRatio="723" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parametros" sheetId="14" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Querys SQL" sheetId="13" state="hidden" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Diccionario Querys'!$A$1:$J$21</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Diccionario Querys'!$A$1:$J$13</definedName>
     <definedName name="periodo_fin">Parametros!$B$6</definedName>
     <definedName name="periodo_inicio">Parametros!$B$7</definedName>
   </definedNames>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="97">
   <si>
     <t>RUT</t>
   </si>
@@ -86,18 +86,6 @@
     <t>CAMPOS FECHAS</t>
   </si>
   <si>
-    <t>FECHA_EFECTO,FECHA_VENCIMIENTO,FINI_RENOV_ANUAL,FFIN_RENOV_ANUAL,FECHA_ANULACION</t>
-  </si>
-  <si>
-    <t>Expuestos Cesantia GES</t>
-  </si>
-  <si>
-    <t>Expuestos Cesantia P10-P12 GES</t>
-  </si>
-  <si>
-    <t>Expuestos Cesantia PR</t>
-  </si>
-  <si>
     <t>Expuestos Desgravamen No Licitado</t>
   </si>
   <si>
@@ -131,9 +119,6 @@
     <t>FEC_NAC,FECHA_EFECTO,FECHA_VENCIMIENTO,FECHA_PREPAGO,FECHA_RENUNCIA,FECHA_FIN_VIGENCIA</t>
   </si>
   <si>
-    <t>FECHA_EFECTO,FECHA_VENCIMIENTO</t>
-  </si>
-  <si>
     <t>FEC_NAC,FECHA_EFECTO,FECHA_VENCIMIENTO,FINI_RENOV_ANUAL,FFIN_RENOV_ANUAL,FECHA_ANULACION</t>
   </si>
   <si>
@@ -161,9 +146,6 @@
     <t>Recargos iAxis</t>
   </si>
   <si>
-    <t>Regiones</t>
-  </si>
-  <si>
     <t>Saldos Insolutos</t>
   </si>
   <si>
@@ -176,9 +158,6 @@
     <t>FECHA_INICIO_RECARGO</t>
   </si>
   <si>
-    <t>FECHA_EFECTO,FECHA_VENCIMIENTO,FFIN_RENOV_ANUAL,FECHA_ANULACION</t>
-  </si>
-  <si>
     <t>Parametros Contrato y Fechas</t>
   </si>
   <si>
@@ -197,12 +176,6 @@
     <t>TIPO EXPORTAR</t>
   </si>
   <si>
-    <t>periodo</t>
-  </si>
-  <si>
-    <t>fecha</t>
-  </si>
-  <si>
     <t>CAMPOS QUERY</t>
   </si>
   <si>
@@ -227,24 +200,15 @@
     <t>POLIZA_SOLICITUD,POLIZA,RUT,SECUENCIAL,PRODUCTO,CODIGO_COBERTURA,VALOR_RECARGO,PORCENTAJE_RECARGO</t>
   </si>
   <si>
-    <t>RUT_CONTRATANTE,CCOMPANI,SSEGURO,POLIZA,CERTIFICADO,PRODUCTO,COD_COB,PLAN_DESC,NRO_OPERACION,TIPO_POLIZA,FECHA_EFECTO,FECHA_VENCIMIENTO,ICAPITAL,IPRIANU,FORMA_PAGO,ESTADO,DESC_ESTADO,REGION,CIUDAD,COMUNA,DIRECCION</t>
-  </si>
-  <si>
     <t>RUT,NRO_OPERACION,POLIZA,SALDO_INSOLUTO</t>
   </si>
   <si>
     <t>RUT,SEXO,FEC_NAC,RUT_CONTRATANTE,CCOMPANI,SSEGURO,POLIZA,CERTIFICADO,PRODUCTO,NRIESGO,COD_COB,PLAN_DESC,NRO_OPERACION,TIPO_POLIZA,FECHA_EFECTO,FECHA_VENCIMIENTO,FECHA_INICIO_CRED,FECHA_FIN_CRED,POLASECFI,POLCFIORI,IPRIANU,FORMA_PAGO,ESTADO,DESC_ESTADO,TASA_CRED,PERIOD_TASA</t>
   </si>
   <si>
-    <t>RUT,SEXO,FEC_NAC,CCOMPANI,SSEGURO,POLIZA,CERTIFICADO,PRODUCTO,COD_COB,PLAN_DESC,NRO_OPERACION,TIPO_POLIZA,FECHA_EFECTO,FECHA_VENCIMIENTO,FECHA_PREPAGO,FECHA_RENUNCIA,FECHA_FIN_VIGENCIA,PERIODO_CONTABILIZACION,ICAPITAL,IPRIANU,FORMA_PAGO,ESTADO,DESC_ESTADO,DESGPRPAG,TASA_CRED,PERIOD_TASA</t>
-  </si>
-  <si>
     <t>Expuestos Desempleo</t>
   </si>
   <si>
-    <t>SSEGURO,POLIZA,CERTIFICADO,PRODUCTO,COD_PLAN,FECHA_EFECTO,FECHA_VENCIMIENTO,FFIN_RENOV_ANUAL,FECHA_ANULACION,REGION,CIUDAD,COMUNA,DIRECCION</t>
-  </si>
-  <si>
     <t>Periodo Fin</t>
   </si>
   <si>
@@ -260,9 +224,6 @@
     <t>K-Fijo</t>
   </si>
   <si>
-    <t>Cesantia PR</t>
-  </si>
-  <si>
     <t>Desgravamen No Licitado</t>
   </si>
   <si>
@@ -359,56 +320,26 @@
     <t>335-10000000</t>
   </si>
   <si>
-    <t>1. Inputs Auxiliares\Regiones I&amp;S</t>
-  </si>
-  <si>
     <t>RUT,SEXO,FEC_NAC,RUT_CONTRATANTE,CCOMPANI,SSEGURO,POLIZA,CERTIFICADO,PRODUCTO,NRIESGO,COD_COB,COD_PLAN,PLAN_DESC,CANAL_VENTA,NRO_RIESGOS,TIPO_POLIZA,FECHA_EFECTO,FECHA_VENCIMIENTO,FINI_RENOV_ANUAL,FFIN_RENOV_ANUAL,FECHA_ANULACION,ICAPITAL,IPRIANU,FORMA_PAGO_CODIGO,ESTADO,DESC_ESTADO</t>
   </si>
   <si>
     <t>RUT,SEXO,FEC_NAC,RUT_CONTRATANTE,CCOMPANI,SSEGURO,POLIZA,CERTIFICADO,PRODUCTO,NRIESGO,COD_COB,COD_PLAN,NRO_RIESGOS,TIPO_POLIZA,FECHA_EFECTO,FECHA_VENCIMIENTO,FECHA_ANULACION,FECHA_CONTABILIZACION_ANULACION,ICAPITAL,IPRIANU,FORMA_PAGO_CODIGO,ESTADO,DESC_ESTADO,TASA_CRED,NCUOTAS,PERIOD_TASA,CTIPREA</t>
   </si>
   <si>
-    <t>RUT_CONTRATANTE,CCOMPANI,SSEGURO,POLIZA,CERTIFICADO,PRODUCTO,COD_COB,COD_PLAN,TIPO_POLIZA,FECHA_EFECTO,FECHA_VENCIMIENTO,FINI_RENOV_ANUAL,FFIN_RENOV_ANUAL,FECHA_ANULACION,ICAPITAL,IPRIANU,FORMA_PAGO_CODIGO,ESTADO,DESC_ESTADO,REGION,CIUDAD,COMUNA,DIRECCION</t>
-  </si>
-  <si>
-    <t>RUT,SEXO,FEC_NAC,RUT_CONTRATANTE,CCOMPANI,SSEGURO,POLIZA,CERTIFICADO,PRODUCTO,NRIESGO,COD_COB,COD_PLAN,TIPO_POLIZA,FECHA_EFECTO,FECHA_VENCIMIENTO,FINI_RENOV_ANUAL,FFIN_RENOV_ANUAL,FECHA_ANULACION,ICAPITAL,IPRIANU,FORMA_PAGO_CODIGO,ESTADO,DESC_ESTADO</t>
-  </si>
-  <si>
-    <t>RUT,SEXO,FEC_NAC,CCOMPANI,SSEGURO,POLIZA,CERTIFICADO,PRODUCTO,COD_COB,COD_PLAN,NRO_OPERACION,TIPO_POLIZA,FECHA_EFECTO,FECHA_VENCIMIENTO,FECHA_ANULACION,FECHA_CONTABILIZACION_ANULACION,ICAPITAL,IPRIANU,FORMA_PAGO_CODIGO,ESTADO,DESC_ESTADO,TASA_CRED,PERIOD_TASA,TIPO_RECIBO</t>
-  </si>
-  <si>
     <t>RUT,SEXO,FEC_NAC,RUT_CONTRATANTE,CCOMPANI,SSEGURO,POLIZA,CERTIFICADO,PRODUCTO,NRIESGO,NRO_OPERACION,COD_COB,COD_PLAN,TIPO_POLIZA,FECHA_EFECTO,FECHA_VENCIMIENTO,FINI_RENOV_ANUAL,FFIN_RENOV_ANUAL,FECHA_ANULACION,ICAPITAL,IPRIANU,FORMA_PAGO_CODIGO,ESTADO,DESC_ESTADO,TASA_CRED,NCUOTAS,PERIOD_TASA</t>
   </si>
   <si>
-    <t>Expuestos Complementario UC</t>
-  </si>
-  <si>
-    <t>Complementario UC</t>
-  </si>
-  <si>
     <t>Cierre</t>
   </si>
   <si>
-    <t>LOB</t>
-  </si>
-  <si>
-    <t>Siniestros de Reaseguro</t>
-  </si>
-  <si>
-    <t>1. Inputs Auxiliares\LOB</t>
-  </si>
-  <si>
-    <t>RUT,SEXO,FEC_NAC,RUT_CONTRATANTE,CCOMPANI,SSEGURO,NRIESGO,POLIZA,CERTIFICADO,PRODUCTO,COD_COB,COD_PLAN,PLAN_DESC,CANAL_VENTA,TIPO_POLIZA,FECHA_EFECTO,FECHA_VENCIMIENTO,FINI_RENOV_ANUAL,FFIN_RENOV_ANUAL,ICAPITAL,IPRIANU,FORMA_PAGO_CODIGO,ESTADO,DESC_ESTADO,MOTIVO_BAJA,SUBMOTIVO_BAJA,FECHA_ANULACION</t>
-  </si>
-  <si>
-    <t>TIPO_REDUCIDO,POLIZA,ENTIDAD,PERIODICIDAD,DESCRIPCION,CLAS_PROFIT,DESC_LOB</t>
+    <t>historico</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -473,13 +404,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -520,7 +444,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -561,20 +485,12 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal_RvaTotGrales_20094_20090429_15_34_Detalle Polizas" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <fill>
-        <patternFill patternType="darkGray"/>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill patternType="darkGray"/>
@@ -888,7 +804,7 @@
   <dimension ref="A4:C7"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:B7"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -900,40 +816,40 @@
   <sheetData>
     <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="B6" s="9">
-        <v>202407</v>
+        <v>202409</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="B7" s="9">
-        <v>202407</v>
+        <v>202409</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -943,10 +859,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:N22"/>
+  <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9:H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -969,31 +885,31 @@
         <v>12</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>13</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
@@ -1002,32 +918,32 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="13" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="F2" s="2">
         <v>0</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>51</v>
+        <v>96</v>
       </c>
       <c r="H2" s="14">
         <v>1</v>
       </c>
       <c r="I2" s="14" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="J2" s="13" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="K2" s="5"/>
       <c r="L2" s="5"/>
@@ -1036,34 +952,34 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>112</v>
+        <v>18</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>113</v>
+        <v>59</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="F3" s="2">
         <v>0</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="H3" s="16">
+        <v>96</v>
+      </c>
+      <c r="H3" s="14">
         <v>1</v>
       </c>
       <c r="I3" s="14" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="J3" s="13" t="s">
-        <v>118</v>
+        <v>93</v>
       </c>
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
@@ -1072,34 +988,34 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H4" s="14">
+        <v>1</v>
+      </c>
+      <c r="I4" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="J4" s="13" t="s">
         <v>94</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F4" s="2">
-        <v>0</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="H4" s="14">
-        <v>1</v>
-      </c>
-      <c r="I4" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="J4" s="13" t="s">
-        <v>107</v>
       </c>
       <c r="K4" s="5"/>
       <c r="L4" s="5"/>
@@ -1108,32 +1024,34 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C5" s="11"/>
+        <v>81</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>83</v>
+      </c>
       <c r="D5" s="13" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="F5" s="2">
         <v>0</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>51</v>
+        <v>96</v>
       </c>
       <c r="H5" s="14">
         <v>1</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="J5" s="13" t="s">
-        <v>108</v>
+        <v>46</v>
       </c>
       <c r="K5" s="5"/>
       <c r="L5" s="5"/>
@@ -1142,34 +1060,32 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>72</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="C6" s="11"/>
       <c r="D6" s="13" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="F6" s="2">
         <v>0</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>51</v>
+        <v>96</v>
       </c>
       <c r="H6" s="14">
         <v>1</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="J6" s="13" t="s">
-        <v>109</v>
+        <v>45</v>
       </c>
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
@@ -1178,32 +1094,32 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>65</v>
+        <v>30</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C7" s="11"/>
-      <c r="D7" s="13" t="s">
-        <v>27</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="D7" s="13"/>
       <c r="E7" s="2" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="F7" s="2">
         <v>0</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>52</v>
+        <v>96</v>
       </c>
       <c r="H7" s="14">
         <v>1</v>
       </c>
       <c r="I7" s="14" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="J7" s="13" t="s">
-        <v>110</v>
+        <v>47</v>
       </c>
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
@@ -1212,34 +1128,34 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="F8" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>51</v>
+        <v>96</v>
       </c>
       <c r="H8" s="14">
         <v>1</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="J8" s="13" t="s">
-        <v>111</v>
+        <v>48</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -1248,34 +1164,34 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="C9" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0</v>
+      </c>
+      <c r="G9" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="D9" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F9" s="2">
-        <v>0</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>51</v>
-      </c>
       <c r="H9" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I9" s="14" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="J9" s="13" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
@@ -1284,34 +1200,32 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>44</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="D10" s="13"/>
       <c r="E10" s="2" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="F10" s="2">
         <v>0</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>51</v>
+        <v>96</v>
       </c>
       <c r="H10" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I10" s="14" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="J10" s="13" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
@@ -1320,14 +1234,16 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" s="13" t="s">
         <v>26</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C11" s="11"/>
-      <c r="D11" s="13" t="s">
-        <v>32</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>9</v>
@@ -1336,16 +1252,16 @@
         <v>0</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>51</v>
+        <v>96</v>
       </c>
       <c r="H11" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I11" s="14" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="J11" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
@@ -1354,13 +1270,13 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="D12" s="13"/>
       <c r="E12" s="2" t="s">
@@ -1370,16 +1286,16 @@
         <v>0</v>
       </c>
       <c r="G12" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H12" s="14">
+        <v>0</v>
+      </c>
+      <c r="I12" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="J12" s="13" t="s">
         <v>51</v>
-      </c>
-      <c r="H12" s="14">
-        <v>1</v>
-      </c>
-      <c r="I12" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="J12" s="13" t="s">
-        <v>56</v>
       </c>
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
@@ -1388,16 +1304,16 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>9</v>
@@ -1406,345 +1322,32 @@
         <v>0</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>51</v>
+        <v>96</v>
       </c>
       <c r="H13" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I13" s="14" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="J13" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
-      <c r="M13" s="4"/>
-      <c r="N13" s="4"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F14" s="2">
-        <v>0</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="H14" s="14">
-        <v>1</v>
-      </c>
-      <c r="I14" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="J14" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="4"/>
-      <c r="N14" s="4"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="D15" s="13"/>
-      <c r="E15" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F15" s="2">
-        <v>2</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="H15" s="14">
-        <v>1</v>
-      </c>
-      <c r="I15" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="J15" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="K15" s="5"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="4"/>
-      <c r="N15" s="4"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C16" s="11"/>
-      <c r="D16" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F16" s="2">
-        <v>0</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="H16" s="14">
-        <v>1</v>
-      </c>
-      <c r="I16" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="J16" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
-      <c r="M16" s="4"/>
-      <c r="N16" s="4"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="D17" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F17" s="2">
-        <v>0</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="H17" s="14">
-        <v>1</v>
-      </c>
-      <c r="I17" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="J17" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
-      <c r="M17" s="4"/>
-      <c r="N17" s="4"/>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="D18" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F18" s="2">
-        <v>2</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="H18" s="14">
-        <v>1</v>
-      </c>
-      <c r="I18" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="J18" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
-      <c r="M18" s="4"/>
-      <c r="N18" s="4"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C19" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="D19" s="13"/>
-      <c r="E19" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F19" s="2">
-        <v>0</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="H19" s="14">
-        <v>1</v>
-      </c>
-      <c r="I19" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="J19" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="K19" s="5"/>
-      <c r="L19" s="5"/>
-      <c r="M19" s="4"/>
-      <c r="N19" s="4"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="D20" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F20" s="2">
-        <v>0</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="H20" s="14">
-        <v>1</v>
-      </c>
-      <c r="I20" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="J20" s="13" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="D21" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F21" s="2">
-        <v>0</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="H21" s="14">
-        <v>1</v>
-      </c>
-      <c r="I21" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="J21" s="13" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="D22" s="13"/>
-      <c r="E22" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F22" s="2">
-        <v>0</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="H22" s="14">
-        <v>1</v>
-      </c>
-      <c r="I22" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="J22" s="13" t="s">
-        <v>119</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A20:D20">
-    <sortCondition ref="A1:A20"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A13:D13">
+    <sortCondition ref="A1:A13"/>
   </sortState>
-  <conditionalFormatting sqref="A2:J21 A21:I22">
-    <cfRule type="expression" dxfId="2" priority="4">
+  <conditionalFormatting sqref="A2:J13">
+    <cfRule type="expression" dxfId="1" priority="4">
       <formula>$H2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J22">
-    <cfRule type="expression" dxfId="1" priority="3">
-      <formula>$H22=0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G22" xr:uid="{306C1357-CD4C-4FDE-AFEC-3E3B64B51A55}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G13" xr:uid="{64581088-80D7-4209-BDBA-76139D2401EB}">
       <formula1>"fecha,periodo,historico"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E22" xr:uid="{5D2AD265-4CC4-42D3-A613-6848219A3908}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E13" xr:uid="{5D2AD265-4CC4-42D3-A613-6848219A3908}">
       <formula1>"GES,IAXIS,IAXIS TEST"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1758,7 +1361,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1774,30 +1377,30 @@
         <v>12</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="D2" s="12"/>
       <c r="E2" s="11">
@@ -1809,85 +1412,85 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="D3" s="12"/>
       <c r="E3" s="11">
         <v>1</v>
       </c>
       <c r="F3" s="15">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="D4" s="12"/>
       <c r="E4" s="11">
         <v>1</v>
       </c>
       <c r="F4" s="15">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="D5" s="12"/>
       <c r="E5" s="11">
         <v>1</v>
       </c>
       <c r="F5" s="15">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="11">
         <v>1</v>
       </c>
       <c r="F6" s="15">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="D7" s="12"/>
       <c r="E7" s="11">
@@ -1899,13 +1502,13 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="11">
@@ -1917,32 +1520,32 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="11">
         <v>1</v>
       </c>
       <c r="F9" s="15">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="C10" s="12"/>
       <c r="D10" s="12" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="E10" s="11">
         <v>0</v>
@@ -1953,14 +1556,14 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="C11" s="12"/>
       <c r="D11" s="12" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="E11" s="11">
         <v>1</v>
@@ -1971,13 +1574,13 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="11">
@@ -1989,13 +1592,13 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="D13" s="12"/>
       <c r="E13" s="11">
@@ -2007,14 +1610,14 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="C14" s="12"/>
       <c r="D14" s="12" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="E14" s="11">
         <v>1</v>
@@ -2025,14 +1628,14 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="C15" s="12"/>
       <c r="D15" s="12" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="E15" s="11">
         <v>0</v>

</xml_diff>